<commit_message>
Passing all the data into the processing and plotting clusters.
</commit_message>
<xml_diff>
--- a/cluster_4.xlsx
+++ b/cluster_4.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhsuh\OneDrive\Desktop\Filtrix\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -8528,8 +8523,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8592,14 +8587,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -8646,7 +8633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8678,10 +8665,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8713,7 +8699,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8889,27 +8874,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.26953125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8941,7 +8913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -8973,7 +8945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -9005,7 +8977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -9037,7 +9009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -9069,7 +9041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -9101,7 +9073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -9133,7 +9105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -9165,7 +9137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -9197,7 +9169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -9229,7 +9201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -9261,7 +9233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -9293,7 +9265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -9325,7 +9297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -9357,7 +9329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -9389,7 +9361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -9421,7 +9393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -9453,7 +9425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -9485,7 +9457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -9517,7 +9489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -9549,7 +9521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -9581,7 +9553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -9613,7 +9585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -9645,7 +9617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -9677,7 +9649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -9709,7 +9681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -9741,7 +9713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -9773,7 +9745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -9805,7 +9777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -9837,7 +9809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -9869,7 +9841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -9901,7 +9873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -9933,7 +9905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -9965,7 +9937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -9997,7 +9969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -10029,7 +10001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -10061,7 +10033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -10093,7 +10065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -10125,7 +10097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -10157,7 +10129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -10189,7 +10161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -10221,7 +10193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -10253,7 +10225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -10285,7 +10257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -10317,7 +10289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -10349,7 +10321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>19</v>
       </c>
@@ -10381,7 +10353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -10413,7 +10385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>19</v>
       </c>
@@ -10445,7 +10417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -10477,7 +10449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>19</v>
       </c>
@@ -10509,7 +10481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -10541,7 +10513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>19</v>
       </c>
@@ -10573,7 +10545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>19</v>
       </c>
@@ -10605,7 +10577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -10637,7 +10609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -10669,7 +10641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -10701,7 +10673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>21</v>
       </c>
@@ -10733,7 +10705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>21</v>
       </c>
@@ -10765,7 +10737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>21</v>
       </c>
@@ -10797,7 +10769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -10829,7 +10801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>21</v>
       </c>
@@ -10861,7 +10833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -10893,7 +10865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -10925,7 +10897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -10957,7 +10929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>21</v>
       </c>
@@ -10989,7 +10961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>21</v>
       </c>
@@ -11021,7 +10993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>21</v>
       </c>
@@ -11053,7 +11025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -11085,7 +11057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>21</v>
       </c>
@@ -11117,7 +11089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -11149,7 +11121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -11181,7 +11153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>17</v>
       </c>
@@ -11213,7 +11185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>21</v>
       </c>
@@ -11245,7 +11217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>21</v>
       </c>
@@ -11277,7 +11249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>21</v>
       </c>
@@ -11309,7 +11281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>21</v>
       </c>
@@ -11341,7 +11313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>21</v>
       </c>
@@ -11373,7 +11345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>21</v>
       </c>
@@ -11405,7 +11377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>21</v>
       </c>
@@ -11437,7 +11409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -11469,7 +11441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>23</v>
       </c>
@@ -11501,7 +11473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -11533,7 +11505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -11565,7 +11537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -11597,7 +11569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -11629,7 +11601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -11661,7 +11633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -11693,7 +11665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -11725,7 +11697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -11757,7 +11729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>17</v>
       </c>
@@ -11789,7 +11761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -11821,7 +11793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -11853,7 +11825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -11885,7 +11857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -11917,7 +11889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -11949,7 +11921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>18</v>
       </c>
@@ -11981,7 +11953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>25</v>
       </c>
@@ -12013,7 +11985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -12045,7 +12017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>25</v>
       </c>
@@ -12077,7 +12049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>25</v>
       </c>
@@ -12109,7 +12081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>25</v>
       </c>
@@ -12141,7 +12113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10">
       <c r="A102" t="s">
         <v>25</v>
       </c>
@@ -12173,7 +12145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10">
       <c r="A103" t="s">
         <v>25</v>
       </c>
@@ -12205,7 +12177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -12237,7 +12209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10">
       <c r="A105" t="s">
         <v>27</v>
       </c>
@@ -12269,7 +12241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10">
       <c r="A106" t="s">
         <v>27</v>
       </c>
@@ -12301,7 +12273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10">
       <c r="A107" t="s">
         <v>27</v>
       </c>
@@ -12333,7 +12305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -12365,7 +12337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10">
       <c r="A109" t="s">
         <v>21</v>
       </c>
@@ -12397,7 +12369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10">
       <c r="A110" t="s">
         <v>21</v>
       </c>
@@ -12429,7 +12401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10">
       <c r="A111" t="s">
         <v>26</v>
       </c>
@@ -12461,7 +12433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10">
       <c r="A112" t="s">
         <v>16</v>
       </c>
@@ -12493,7 +12465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10">
       <c r="A113" t="s">
         <v>21</v>
       </c>
@@ -12525,7 +12497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10">
       <c r="A114" t="s">
         <v>22</v>
       </c>
@@ -12557,7 +12529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10">
       <c r="A115" t="s">
         <v>22</v>
       </c>
@@ -12589,7 +12561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10">
       <c r="A116" t="s">
         <v>21</v>
       </c>
@@ -12621,7 +12593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10">
       <c r="A117" t="s">
         <v>21</v>
       </c>
@@ -12653,7 +12625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10">
       <c r="A118" t="s">
         <v>22</v>
       </c>
@@ -12685,7 +12657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10">
       <c r="A119" t="s">
         <v>21</v>
       </c>
@@ -12717,7 +12689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10">
       <c r="A120" t="s">
         <v>22</v>
       </c>
@@ -12749,7 +12721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10">
       <c r="A121" t="s">
         <v>21</v>
       </c>
@@ -12781,7 +12753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10">
       <c r="A122" t="s">
         <v>21</v>
       </c>
@@ -12813,7 +12785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10">
       <c r="A123" t="s">
         <v>21</v>
       </c>
@@ -12845,7 +12817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10">
       <c r="A124" t="s">
         <v>21</v>
       </c>
@@ -12877,7 +12849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10">
       <c r="A125" t="s">
         <v>22</v>
       </c>
@@ -12909,7 +12881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10">
       <c r="A126" t="s">
         <v>27</v>
       </c>
@@ -12941,7 +12913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10">
       <c r="A127" t="s">
         <v>21</v>
       </c>
@@ -12973,7 +12945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10">
       <c r="A128" t="s">
         <v>22</v>
       </c>
@@ -13005,7 +12977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10">
       <c r="A129" t="s">
         <v>22</v>
       </c>
@@ -13037,7 +13009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10">
       <c r="A130" t="s">
         <v>22</v>
       </c>
@@ -13069,7 +13041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10">
       <c r="A131" t="s">
         <v>21</v>
       </c>
@@ -13101,7 +13073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10">
       <c r="A132" t="s">
         <v>21</v>
       </c>
@@ -13133,7 +13105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10">
       <c r="A133" t="s">
         <v>22</v>
       </c>
@@ -13165,7 +13137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10">
       <c r="A134" t="s">
         <v>22</v>
       </c>
@@ -13197,7 +13169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10">
       <c r="A135" t="s">
         <v>21</v>
       </c>
@@ -13229,7 +13201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10">
       <c r="A136" t="s">
         <v>21</v>
       </c>
@@ -13261,7 +13233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10">
       <c r="A137" t="s">
         <v>21</v>
       </c>
@@ -13293,7 +13265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10">
       <c r="A138" t="s">
         <v>21</v>
       </c>
@@ -13325,7 +13297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10">
       <c r="A139" t="s">
         <v>21</v>
       </c>
@@ -13357,7 +13329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10">
       <c r="A140" t="s">
         <v>21</v>
       </c>
@@ -13389,7 +13361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10">
       <c r="A141" t="s">
         <v>21</v>
       </c>
@@ -13421,7 +13393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10">
       <c r="A142" t="s">
         <v>21</v>
       </c>
@@ -13453,7 +13425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10">
       <c r="A143" t="s">
         <v>22</v>
       </c>
@@ -13485,7 +13457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10">
       <c r="A144" t="s">
         <v>21</v>
       </c>
@@ -13517,7 +13489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10">
       <c r="A145" t="s">
         <v>27</v>
       </c>
@@ -13549,7 +13521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10">
       <c r="A146" t="s">
         <v>26</v>
       </c>
@@ -13581,7 +13553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10">
       <c r="A147" t="s">
         <v>28</v>
       </c>
@@ -13613,7 +13585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10">
       <c r="A148" t="s">
         <v>13</v>
       </c>
@@ -13645,7 +13617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10">
       <c r="A149" t="s">
         <v>29</v>
       </c>
@@ -13677,7 +13649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10">
       <c r="A150" t="s">
         <v>30</v>
       </c>
@@ -13709,7 +13681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -13741,7 +13713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -13773,7 +13745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10">
       <c r="A153" t="s">
         <v>29</v>
       </c>
@@ -13805,7 +13777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10">
       <c r="A154" t="s">
         <v>31</v>
       </c>
@@ -13837,7 +13809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -13869,7 +13841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -13901,7 +13873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10">
       <c r="A157" t="s">
         <v>29</v>
       </c>
@@ -13933,7 +13905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -13965,7 +13937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10">
       <c r="A159" t="s">
         <v>32</v>
       </c>
@@ -13997,7 +13969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10">
       <c r="A160" t="s">
         <v>29</v>
       </c>
@@ -14029,7 +14001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -14061,7 +14033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10">
       <c r="A162" t="s">
         <v>33</v>
       </c>
@@ -14093,7 +14065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10">
       <c r="A163" t="s">
         <v>33</v>
       </c>
@@ -14125,7 +14097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10">
       <c r="A164" t="s">
         <v>34</v>
       </c>
@@ -14157,7 +14129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -14189,7 +14161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10">
       <c r="A166" t="s">
         <v>33</v>
       </c>
@@ -14221,7 +14193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -14253,7 +14225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10">
       <c r="A168" t="s">
         <v>35</v>
       </c>
@@ -14285,7 +14257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10">
       <c r="A169" t="s">
         <v>35</v>
       </c>
@@ -14317,7 +14289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10">
       <c r="A170" t="s">
         <v>35</v>
       </c>
@@ -14349,7 +14321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10">
       <c r="A171" t="s">
         <v>35</v>
       </c>
@@ -14381,7 +14353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10">
       <c r="A172" t="s">
         <v>35</v>
       </c>
@@ -14413,7 +14385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10">
       <c r="A173" t="s">
         <v>35</v>
       </c>
@@ -14445,7 +14417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10">
       <c r="A174" t="s">
         <v>35</v>
       </c>
@@ -14477,7 +14449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10">
       <c r="A175" t="s">
         <v>36</v>
       </c>
@@ -14509,7 +14481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10">
       <c r="A176" t="s">
         <v>35</v>
       </c>
@@ -14541,7 +14513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10">
       <c r="A177" t="s">
         <v>35</v>
       </c>
@@ -14573,7 +14545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10">
       <c r="A178" t="s">
         <v>35</v>
       </c>
@@ -14605,7 +14577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10">
       <c r="A179" t="s">
         <v>35</v>
       </c>
@@ -14637,7 +14609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10">
       <c r="A180" t="s">
         <v>35</v>
       </c>
@@ -14669,7 +14641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10">
       <c r="A181" t="s">
         <v>34</v>
       </c>
@@ -14701,7 +14673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10">
       <c r="A182" t="s">
         <v>35</v>
       </c>
@@ -14733,7 +14705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10">
       <c r="A183" t="s">
         <v>35</v>
       </c>
@@ -14765,7 +14737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10">
       <c r="A184" t="s">
         <v>35</v>
       </c>
@@ -14797,7 +14769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10">
       <c r="A185" t="s">
         <v>35</v>
       </c>
@@ -14829,7 +14801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10">
       <c r="A186" t="s">
         <v>35</v>
       </c>
@@ -14861,7 +14833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10">
       <c r="A187" t="s">
         <v>35</v>
       </c>
@@ -14893,7 +14865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10">
       <c r="A188" t="s">
         <v>35</v>
       </c>
@@ -14925,7 +14897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10">
       <c r="A189" t="s">
         <v>35</v>
       </c>
@@ -14957,7 +14929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10">
       <c r="A190" t="s">
         <v>35</v>
       </c>
@@ -14989,7 +14961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10">
       <c r="A191" t="s">
         <v>35</v>
       </c>
@@ -15021,7 +14993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10">
       <c r="A192" t="s">
         <v>35</v>
       </c>
@@ -15053,7 +15025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10">
       <c r="A193" t="s">
         <v>35</v>
       </c>
@@ -15085,7 +15057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10">
       <c r="A194" t="s">
         <v>35</v>
       </c>
@@ -15117,7 +15089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10">
       <c r="A195" t="s">
         <v>36</v>
       </c>
@@ -15149,7 +15121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10">
       <c r="A196" t="s">
         <v>35</v>
       </c>
@@ -15181,7 +15153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10">
       <c r="A197" t="s">
         <v>35</v>
       </c>
@@ -15213,7 +15185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10">
       <c r="A198" t="s">
         <v>35</v>
       </c>
@@ -15245,7 +15217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10">
       <c r="A199" t="s">
         <v>36</v>
       </c>
@@ -15277,7 +15249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10">
       <c r="A200" t="s">
         <v>35</v>
       </c>
@@ -15309,7 +15281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10">
       <c r="A201" t="s">
         <v>35</v>
       </c>
@@ -15341,7 +15313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10">
       <c r="A202" t="s">
         <v>35</v>
       </c>
@@ -15373,7 +15345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10">
       <c r="A203" t="s">
         <v>35</v>
       </c>
@@ -15405,7 +15377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10">
       <c r="A204" t="s">
         <v>35</v>
       </c>
@@ -15437,7 +15409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10">
       <c r="A205" t="s">
         <v>35</v>
       </c>
@@ -15469,7 +15441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10">
       <c r="A206" t="s">
         <v>35</v>
       </c>
@@ -15501,7 +15473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10">
       <c r="A207" t="s">
         <v>35</v>
       </c>
@@ -15533,7 +15505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10">
       <c r="A208" t="s">
         <v>35</v>
       </c>
@@ -15565,7 +15537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:10">
       <c r="A209" t="s">
         <v>36</v>
       </c>
@@ -15597,7 +15569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:10">
       <c r="A210" t="s">
         <v>35</v>
       </c>
@@ -15629,7 +15601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:10">
       <c r="A211" t="s">
         <v>35</v>
       </c>
@@ -15661,7 +15633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:10">
       <c r="A212" t="s">
         <v>36</v>
       </c>
@@ -15693,7 +15665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:10">
       <c r="A213" t="s">
         <v>35</v>
       </c>
@@ -15725,7 +15697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:10">
       <c r="A214" t="s">
         <v>35</v>
       </c>
@@ -15757,7 +15729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10">
       <c r="A215" t="s">
         <v>35</v>
       </c>
@@ -15789,7 +15761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:10">
       <c r="A216" t="s">
         <v>36</v>
       </c>
@@ -15821,7 +15793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:10">
       <c r="A217" t="s">
         <v>37</v>
       </c>
@@ -15853,7 +15825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10">
       <c r="A218" t="s">
         <v>10</v>
       </c>
@@ -15885,7 +15857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10">
       <c r="A219" t="s">
         <v>33</v>
       </c>
@@ -15917,7 +15889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10">
       <c r="A220" t="s">
         <v>35</v>
       </c>
@@ -15949,7 +15921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10">
       <c r="A221" t="s">
         <v>35</v>
       </c>
@@ -15981,7 +15953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10">
       <c r="A222" t="s">
         <v>35</v>
       </c>
@@ -16013,7 +15985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10">
       <c r="A223" t="s">
         <v>36</v>
       </c>
@@ -16045,7 +16017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10">
       <c r="A224" t="s">
         <v>10</v>
       </c>
@@ -16077,7 +16049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10">
       <c r="A225" t="s">
         <v>35</v>
       </c>
@@ -16109,7 +16081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10">
       <c r="A226" t="s">
         <v>10</v>
       </c>
@@ -16141,7 +16113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10">
       <c r="A227" t="s">
         <v>35</v>
       </c>
@@ -16173,7 +16145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10">
       <c r="A228" t="s">
         <v>36</v>
       </c>
@@ -16205,7 +16177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10">
       <c r="A229" t="s">
         <v>35</v>
       </c>
@@ -16237,7 +16209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10">
       <c r="A230" t="s">
         <v>35</v>
       </c>
@@ -16269,7 +16241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10">
       <c r="A231" t="s">
         <v>35</v>
       </c>
@@ -16301,7 +16273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10">
       <c r="A232" t="s">
         <v>35</v>
       </c>
@@ -16333,7 +16305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10">
       <c r="A233" t="s">
         <v>35</v>
       </c>
@@ -16365,7 +16337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10">
       <c r="A234" t="s">
         <v>36</v>
       </c>
@@ -16397,7 +16369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10">
       <c r="A235" t="s">
         <v>35</v>
       </c>
@@ -16429,7 +16401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10">
       <c r="A236" t="s">
         <v>35</v>
       </c>
@@ -16461,7 +16433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10">
       <c r="A237" t="s">
         <v>35</v>
       </c>
@@ -16493,7 +16465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10">
       <c r="A238" t="s">
         <v>35</v>
       </c>
@@ -16525,7 +16497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10">
       <c r="A239" t="s">
         <v>35</v>
       </c>
@@ -16557,7 +16529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10">
       <c r="A240" t="s">
         <v>35</v>
       </c>
@@ -16589,7 +16561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10">
       <c r="A241" t="s">
         <v>35</v>
       </c>
@@ -16621,7 +16593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10">
       <c r="A242" t="s">
         <v>38</v>
       </c>
@@ -16653,7 +16625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10">
       <c r="A243" t="s">
         <v>35</v>
       </c>
@@ -16685,7 +16657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10">
       <c r="A244" t="s">
         <v>35</v>
       </c>
@@ -16717,7 +16689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10">
       <c r="A245" t="s">
         <v>35</v>
       </c>
@@ -16749,7 +16721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10">
       <c r="A246" t="s">
         <v>35</v>
       </c>
@@ -16781,7 +16753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10">
       <c r="A247" t="s">
         <v>35</v>
       </c>
@@ -16813,7 +16785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10">
       <c r="A248" t="s">
         <v>39</v>
       </c>
@@ -16845,7 +16817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10">
       <c r="A249" t="s">
         <v>39</v>
       </c>
@@ -16877,7 +16849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10">
       <c r="A250" t="s">
         <v>37</v>
       </c>
@@ -16909,7 +16881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10">
       <c r="A251" t="s">
         <v>40</v>
       </c>
@@ -16941,7 +16913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10">
       <c r="A252" t="s">
         <v>39</v>
       </c>
@@ -16973,7 +16945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10">
       <c r="A253" t="s">
         <v>39</v>
       </c>
@@ -17005,7 +16977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10">
       <c r="A254" t="s">
         <v>40</v>
       </c>
@@ -17037,7 +17009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10">
       <c r="A255" t="s">
         <v>41</v>
       </c>
@@ -17069,7 +17041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10">
       <c r="A256" t="s">
         <v>39</v>
       </c>
@@ -17101,7 +17073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10">
       <c r="A257" t="s">
         <v>42</v>
       </c>
@@ -17133,7 +17105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10">
       <c r="A258" t="s">
         <v>39</v>
       </c>
@@ -17165,7 +17137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10">
       <c r="A259" t="s">
         <v>39</v>
       </c>
@@ -17197,7 +17169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10">
       <c r="A260" t="s">
         <v>39</v>
       </c>
@@ -17229,7 +17201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10">
       <c r="A261" t="s">
         <v>39</v>
       </c>
@@ -17261,7 +17233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10">
       <c r="A262" t="s">
         <v>39</v>
       </c>
@@ -17293,7 +17265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10">
       <c r="A263" t="s">
         <v>39</v>
       </c>
@@ -17325,7 +17297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10">
       <c r="A264" t="s">
         <v>39</v>
       </c>
@@ -17357,7 +17329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10">
       <c r="A265" t="s">
         <v>40</v>
       </c>
@@ -17389,7 +17361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10">
       <c r="A266" t="s">
         <v>39</v>
       </c>
@@ -17421,7 +17393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10">
       <c r="A267" t="s">
         <v>39</v>
       </c>
@@ -17453,7 +17425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10">
       <c r="A268" t="s">
         <v>39</v>
       </c>
@@ -17485,7 +17457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10">
       <c r="A269" t="s">
         <v>39</v>
       </c>
@@ -17517,7 +17489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10">
       <c r="A270" t="s">
         <v>39</v>
       </c>
@@ -17549,7 +17521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10">
       <c r="A271" t="s">
         <v>39</v>
       </c>
@@ -17581,7 +17553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10">
       <c r="A272" t="s">
         <v>39</v>
       </c>
@@ -17613,7 +17585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10">
       <c r="A273" t="s">
         <v>39</v>
       </c>
@@ -17645,7 +17617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10">
       <c r="A274" t="s">
         <v>39</v>
       </c>
@@ -17677,7 +17649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10">
       <c r="A275" t="s">
         <v>39</v>
       </c>
@@ -17709,7 +17681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10">
       <c r="A276" t="s">
         <v>40</v>
       </c>
@@ -17741,7 +17713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10">
       <c r="A277" t="s">
         <v>43</v>
       </c>
@@ -17773,7 +17745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10">
       <c r="A278" t="s">
         <v>39</v>
       </c>
@@ -17805,7 +17777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10">
       <c r="A279" t="s">
         <v>39</v>
       </c>
@@ -17837,7 +17809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10">
       <c r="A280" t="s">
         <v>39</v>
       </c>
@@ -17869,7 +17841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10">
       <c r="A281" t="s">
         <v>40</v>
       </c>
@@ -17901,7 +17873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10">
       <c r="A282" t="s">
         <v>39</v>
       </c>
@@ -17933,7 +17905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10">
       <c r="A283" t="s">
         <v>39</v>
       </c>
@@ -17965,7 +17937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10">
       <c r="A284" t="s">
         <v>39</v>
       </c>
@@ -17997,7 +17969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10">
       <c r="A285" t="s">
         <v>39</v>
       </c>
@@ -18029,7 +18001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10">
       <c r="A286" t="s">
         <v>39</v>
       </c>
@@ -18061,7 +18033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10">
       <c r="A287" t="s">
         <v>39</v>
       </c>
@@ -18093,7 +18065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10">
       <c r="A288" t="s">
         <v>44</v>
       </c>
@@ -18125,7 +18097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10">
       <c r="A289" t="s">
         <v>39</v>
       </c>
@@ -18157,7 +18129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10">
       <c r="A290" t="s">
         <v>39</v>
       </c>
@@ -18189,7 +18161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10">
       <c r="A291" t="s">
         <v>39</v>
       </c>
@@ -18221,7 +18193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:10">
       <c r="A292" t="s">
         <v>45</v>
       </c>
@@ -18253,7 +18225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:10">
       <c r="A293" t="s">
         <v>40</v>
       </c>
@@ -18285,7 +18257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10">
       <c r="A294" t="s">
         <v>39</v>
       </c>
@@ -18317,7 +18289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:10">
       <c r="A295" t="s">
         <v>39</v>
       </c>
@@ -18349,7 +18321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10">
       <c r="A296" t="s">
         <v>39</v>
       </c>
@@ -18381,7 +18353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10">
       <c r="A297" t="s">
         <v>40</v>
       </c>
@@ -18413,7 +18385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10">
       <c r="A298" t="s">
         <v>39</v>
       </c>
@@ -18445,7 +18417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10">
       <c r="A299" t="s">
         <v>39</v>
       </c>
@@ -18477,7 +18449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10">
       <c r="A300" t="s">
         <v>39</v>
       </c>
@@ -18509,7 +18481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10">
       <c r="A301" t="s">
         <v>39</v>
       </c>
@@ -18541,7 +18513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:10">
       <c r="A302" t="s">
         <v>39</v>
       </c>
@@ -18573,7 +18545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:10">
       <c r="A303" t="s">
         <v>39</v>
       </c>
@@ -18605,7 +18577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:10">
       <c r="A304" t="s">
         <v>39</v>
       </c>
@@ -18637,7 +18609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:10">
       <c r="A305" t="s">
         <v>40</v>
       </c>
@@ -18669,7 +18641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:10">
       <c r="A306" t="s">
         <v>46</v>
       </c>
@@ -18701,7 +18673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:10">
       <c r="A307" t="s">
         <v>39</v>
       </c>
@@ -18733,7 +18705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:10">
       <c r="A308" t="s">
         <v>39</v>
       </c>
@@ -18765,7 +18737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:10">
       <c r="A309" t="s">
         <v>39</v>
       </c>
@@ -18797,7 +18769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:10">
       <c r="A310" t="s">
         <v>39</v>
       </c>
@@ -18829,7 +18801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:10">
       <c r="A311" t="s">
         <v>40</v>
       </c>
@@ -18861,7 +18833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:10">
       <c r="A312" t="s">
         <v>43</v>
       </c>
@@ -18893,7 +18865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:10">
       <c r="A313" t="s">
         <v>39</v>
       </c>
@@ -18925,7 +18897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:10">
       <c r="A314" t="s">
         <v>39</v>
       </c>
@@ -18957,7 +18929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:10">
       <c r="A315" t="s">
         <v>39</v>
       </c>
@@ -18989,7 +18961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:10">
       <c r="A316" t="s">
         <v>39</v>
       </c>
@@ -19021,7 +18993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:10">
       <c r="A317" t="s">
         <v>39</v>
       </c>
@@ -19053,7 +19025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:10">
       <c r="A318" t="s">
         <v>39</v>
       </c>
@@ -19085,7 +19057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:10">
       <c r="A319" t="s">
         <v>39</v>
       </c>
@@ -19117,7 +19089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:10">
       <c r="A320" t="s">
         <v>39</v>
       </c>
@@ -19149,7 +19121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:10">
       <c r="A321" t="s">
         <v>40</v>
       </c>
@@ -19181,7 +19153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:10">
       <c r="A322" t="s">
         <v>39</v>
       </c>
@@ -19213,7 +19185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:10">
       <c r="A323" t="s">
         <v>39</v>
       </c>
@@ -19245,7 +19217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:10">
       <c r="A324" t="s">
         <v>43</v>
       </c>
@@ -19277,7 +19249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:10">
       <c r="A325" t="s">
         <v>39</v>
       </c>
@@ -19309,7 +19281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:10">
       <c r="A326" t="s">
         <v>39</v>
       </c>
@@ -19341,7 +19313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:10">
       <c r="A327" t="s">
         <v>39</v>
       </c>
@@ -19373,7 +19345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:10">
       <c r="A328" t="s">
         <v>40</v>
       </c>
@@ -19405,7 +19377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:10">
       <c r="A329" t="s">
         <v>39</v>
       </c>
@@ -19437,7 +19409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:10">
       <c r="A330" t="s">
         <v>39</v>
       </c>
@@ -19469,7 +19441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:10">
       <c r="A331" t="s">
         <v>39</v>
       </c>
@@ -19501,7 +19473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:10">
       <c r="A332" t="s">
         <v>39</v>
       </c>
@@ -19533,7 +19505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:10">
       <c r="A333" t="s">
         <v>40</v>
       </c>
@@ -19565,7 +19537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:10">
       <c r="A334" t="s">
         <v>39</v>
       </c>
@@ -19597,7 +19569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:10">
       <c r="A335" t="s">
         <v>39</v>
       </c>
@@ -19629,7 +19601,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:10">
       <c r="A336" t="s">
         <v>43</v>
       </c>
@@ -19661,7 +19633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:10">
       <c r="A337" t="s">
         <v>39</v>
       </c>
@@ -19693,7 +19665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:10">
       <c r="A338" t="s">
         <v>39</v>
       </c>
@@ -19725,7 +19697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:10">
       <c r="A339" t="s">
         <v>39</v>
       </c>
@@ -19757,7 +19729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:10">
       <c r="A340" t="s">
         <v>39</v>
       </c>
@@ -19789,7 +19761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:10">
       <c r="A341" t="s">
         <v>40</v>
       </c>
@@ -19821,7 +19793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:10">
       <c r="A342" t="s">
         <v>42</v>
       </c>
@@ -19853,7 +19825,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:10">
       <c r="A343" t="s">
         <v>39</v>
       </c>
@@ -19885,7 +19857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:10">
       <c r="A344" t="s">
         <v>39</v>
       </c>
@@ -19917,7 +19889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:10">
       <c r="A345" t="s">
         <v>39</v>
       </c>
@@ -19949,7 +19921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:10">
       <c r="A346" t="s">
         <v>39</v>
       </c>
@@ -19981,7 +19953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:10">
       <c r="A347" t="s">
         <v>39</v>
       </c>
@@ -20013,7 +19985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:10">
       <c r="A348" t="s">
         <v>39</v>
       </c>
@@ -20045,7 +20017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:10">
       <c r="A349" t="s">
         <v>39</v>
       </c>
@@ -20077,7 +20049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:10">
       <c r="A350" t="s">
         <v>39</v>
       </c>
@@ -20109,7 +20081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:10">
       <c r="A351" t="s">
         <v>40</v>
       </c>
@@ -20141,7 +20113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:10">
       <c r="A352" t="s">
         <v>39</v>
       </c>
@@ -20173,7 +20145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:10">
       <c r="A353" t="s">
         <v>39</v>
       </c>
@@ -20205,7 +20177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:10">
       <c r="A354" t="s">
         <v>39</v>
       </c>
@@ -20237,7 +20209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:10">
       <c r="A355" t="s">
         <v>40</v>
       </c>
@@ -20269,7 +20241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:10">
       <c r="A356" t="s">
         <v>47</v>
       </c>
@@ -20301,7 +20273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:10">
       <c r="A357" t="s">
         <v>44</v>
       </c>
@@ -20333,7 +20305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:10">
       <c r="A358" t="s">
         <v>42</v>
       </c>
@@ -20365,7 +20337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:10">
       <c r="A359" t="s">
         <v>39</v>
       </c>
@@ -20397,7 +20369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:10">
       <c r="A360" t="s">
         <v>39</v>
       </c>
@@ -20429,7 +20401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:10">
       <c r="A361" t="s">
         <v>39</v>
       </c>
@@ -20461,7 +20433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:10">
       <c r="A362" t="s">
         <v>40</v>
       </c>
@@ -20493,7 +20465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:10">
       <c r="A363" t="s">
         <v>39</v>
       </c>
@@ -20525,7 +20497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:10">
       <c r="A364" t="s">
         <v>39</v>
       </c>
@@ -20557,7 +20529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:10">
       <c r="A365" t="s">
         <v>39</v>
       </c>
@@ -20589,7 +20561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:10">
       <c r="A366" t="s">
         <v>40</v>
       </c>
@@ -20621,7 +20593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:10">
       <c r="A367" t="s">
         <v>39</v>
       </c>
@@ -20653,7 +20625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:10">
       <c r="A368" t="s">
         <v>39</v>
       </c>
@@ -20685,7 +20657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:10">
       <c r="A369" t="s">
         <v>40</v>
       </c>
@@ -20717,7 +20689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:10">
       <c r="A370" t="s">
         <v>39</v>
       </c>
@@ -20749,7 +20721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:10">
       <c r="A371" t="s">
         <v>39</v>
       </c>
@@ -20781,7 +20753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:10">
       <c r="A372" t="s">
         <v>40</v>
       </c>
@@ -20813,7 +20785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:10">
       <c r="A373" t="s">
         <v>39</v>
       </c>
@@ -20845,7 +20817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:10">
       <c r="A374" t="s">
         <v>48</v>
       </c>
@@ -20877,7 +20849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:10">
       <c r="A375" t="s">
         <v>39</v>
       </c>
@@ -20909,7 +20881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:10">
       <c r="A376" t="s">
         <v>40</v>
       </c>
@@ -20941,7 +20913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:10">
       <c r="A377" t="s">
         <v>39</v>
       </c>
@@ -20973,7 +20945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:10">
       <c r="A378" t="s">
         <v>39</v>
       </c>
@@ -21005,7 +20977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:10">
       <c r="A379" t="s">
         <v>40</v>
       </c>
@@ -21037,7 +21009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:10">
       <c r="A380" t="s">
         <v>42</v>
       </c>
@@ -21069,7 +21041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:10">
       <c r="A381" t="s">
         <v>48</v>
       </c>
@@ -21101,7 +21073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:10">
       <c r="A382" t="s">
         <v>48</v>
       </c>
@@ -21133,7 +21105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:10">
       <c r="A383" t="s">
         <v>39</v>
       </c>
@@ -21165,7 +21137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:10">
       <c r="A384" t="s">
         <v>39</v>
       </c>
@@ -21197,7 +21169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:10">
       <c r="A385" t="s">
         <v>39</v>
       </c>
@@ -21229,7 +21201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:10">
       <c r="A386" t="s">
         <v>39</v>
       </c>
@@ -21261,7 +21233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:10">
       <c r="A387" t="s">
         <v>39</v>
       </c>
@@ -21293,7 +21265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:10">
       <c r="A388" t="s">
         <v>40</v>
       </c>
@@ -21325,7 +21297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:10">
       <c r="A389" t="s">
         <v>39</v>
       </c>
@@ -21357,7 +21329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:10">
       <c r="A390" t="s">
         <v>39</v>
       </c>
@@ -21389,7 +21361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:10">
       <c r="A391" t="s">
         <v>39</v>
       </c>
@@ -21421,7 +21393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:10">
       <c r="A392" t="s">
         <v>40</v>
       </c>
@@ -21453,7 +21425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:10">
       <c r="A393" t="s">
         <v>39</v>
       </c>
@@ -21485,7 +21457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:10">
       <c r="A394" t="s">
         <v>39</v>
       </c>
@@ -21517,7 +21489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:10">
       <c r="A395" t="s">
         <v>40</v>
       </c>
@@ -21549,7 +21521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:10">
       <c r="A396" t="s">
         <v>39</v>
       </c>
@@ -21581,7 +21553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:10">
       <c r="A397" t="s">
         <v>39</v>
       </c>
@@ -21613,7 +21585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:10">
       <c r="A398" t="s">
         <v>39</v>
       </c>
@@ -21645,7 +21617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:10">
       <c r="A399" t="s">
         <v>40</v>
       </c>
@@ -21677,7 +21649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:10">
       <c r="A400" t="s">
         <v>39</v>
       </c>
@@ -21709,7 +21681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:10">
       <c r="A401" t="s">
         <v>39</v>
       </c>
@@ -21741,7 +21713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:10">
       <c r="A402" t="s">
         <v>44</v>
       </c>
@@ -21773,7 +21745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:10">
       <c r="A403" t="s">
         <v>39</v>
       </c>
@@ -21805,7 +21777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:10">
       <c r="A404" t="s">
         <v>39</v>
       </c>
@@ -21837,7 +21809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:10">
       <c r="A405" t="s">
         <v>39</v>
       </c>
@@ -21869,7 +21841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:10">
       <c r="A406" t="s">
         <v>39</v>
       </c>
@@ -21901,7 +21873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:10">
       <c r="A407" t="s">
         <v>40</v>
       </c>
@@ -21933,7 +21905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:10">
       <c r="A408" t="s">
         <v>39</v>
       </c>
@@ -21965,7 +21937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:10">
       <c r="A409" t="s">
         <v>39</v>
       </c>
@@ -21997,7 +21969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:10">
       <c r="A410" t="s">
         <v>40</v>
       </c>
@@ -22029,7 +22001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:10">
       <c r="A411" t="s">
         <v>39</v>
       </c>
@@ -22061,7 +22033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:10">
       <c r="A412" t="s">
         <v>47</v>
       </c>
@@ -22093,7 +22065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:10">
       <c r="A413" t="s">
         <v>39</v>
       </c>
@@ -22125,7 +22097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:10">
       <c r="A414" t="s">
         <v>40</v>
       </c>
@@ -22157,7 +22129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:10">
       <c r="A415" t="s">
         <v>41</v>
       </c>
@@ -22189,7 +22161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:10">
       <c r="A416" t="s">
         <v>39</v>
       </c>
@@ -22221,7 +22193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:10">
       <c r="A417" t="s">
         <v>39</v>
       </c>
@@ -22253,7 +22225,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:10">
       <c r="A418" t="s">
         <v>42</v>
       </c>
@@ -22285,7 +22257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:10">
       <c r="A419" t="s">
         <v>39</v>
       </c>
@@ -22317,7 +22289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:10">
       <c r="A420" t="s">
         <v>39</v>
       </c>
@@ -22349,7 +22321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:10">
       <c r="A421" t="s">
         <v>39</v>
       </c>
@@ -22381,7 +22353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:10">
       <c r="A422" t="s">
         <v>40</v>
       </c>
@@ -22413,7 +22385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:10">
       <c r="A423" t="s">
         <v>39</v>
       </c>
@@ -22445,7 +22417,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:10">
       <c r="A424" t="s">
         <v>39</v>
       </c>
@@ -22477,7 +22449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:10">
       <c r="A425" t="s">
         <v>40</v>
       </c>
@@ -22509,7 +22481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:10">
       <c r="A426" t="s">
         <v>39</v>
       </c>
@@ -22541,7 +22513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:10">
       <c r="A427" t="s">
         <v>49</v>
       </c>
@@ -22573,7 +22545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:10">
       <c r="A428" t="s">
         <v>39</v>
       </c>
@@ -22605,7 +22577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:10">
       <c r="A429" t="s">
         <v>40</v>
       </c>
@@ -22637,7 +22609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:10">
       <c r="A430" t="s">
         <v>39</v>
       </c>
@@ -22669,7 +22641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:10">
       <c r="A431" t="s">
         <v>39</v>
       </c>
@@ -22701,7 +22673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:10">
       <c r="A432" t="s">
         <v>39</v>
       </c>
@@ -22733,7 +22705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:10">
       <c r="A433" t="s">
         <v>39</v>
       </c>
@@ -22765,7 +22737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:10">
       <c r="A434" t="s">
         <v>39</v>
       </c>
@@ -22797,7 +22769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:10">
       <c r="A435" t="s">
         <v>40</v>
       </c>
@@ -22829,7 +22801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:10">
       <c r="A436" t="s">
         <v>39</v>
       </c>
@@ -22861,7 +22833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:10">
       <c r="A437" t="s">
         <v>39</v>
       </c>
@@ -22893,7 +22865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:10">
       <c r="A438" t="s">
         <v>41</v>
       </c>
@@ -22925,7 +22897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:10">
       <c r="A439" t="s">
         <v>39</v>
       </c>
@@ -22957,7 +22929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:10">
       <c r="A440" t="s">
         <v>48</v>
       </c>
@@ -22989,7 +22961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:10">
       <c r="A441" t="s">
         <v>39</v>
       </c>

</xml_diff>